<commit_message>
Test cases added to Jira
</commit_message>
<xml_diff>
--- a/SwagLabs_TestCases_Template.xlsx
+++ b/SwagLabs_TestCases_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MTsonkova\MyFiles\Projects\SwagLabs-Testing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA4B5A6-E75A-429D-AD93-89BA023DC5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F7ED37-D9B6-4F3A-A041-6B7F7B7EAC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>Warning message "Epic sadface: Sorry, this user has been locked out." appears.</t>
   </si>
   <si>
-    <t>Log in with invalid credentials that are restricted.</t>
-  </si>
-  <si>
     <t>Login with username and password that are not registered in the database.</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>Badge icon over the shopping cart when removing a product.</t>
   </si>
   <si>
-    <t>Badge icon over the shopping cart when removig all products and the cart is empty.</t>
-  </si>
-  <si>
     <t>Add product to the Shopping Cart from products page.</t>
   </si>
   <si>
@@ -581,12 +575,6 @@
 4. Press Continue button.</t>
   </si>
   <si>
-    <t>1. Enter valid data in First Name field.
-2. Enter valid data in Last Name field.
-3. Leave Zip/Postal Code field empty.
-4. PressContinue button.</t>
-  </si>
-  <si>
     <t>1.Enter vaid data in First Name field.
 2. Enter valid data in Last Name field.
 3. Enter valid data in the Zip/Postal Code field.
@@ -682,9 +670,6 @@
   </si>
   <si>
     <t>User is redirected to Products Page</t>
-  </si>
-  <si>
-    <t>SW033</t>
   </si>
   <si>
     <t>User logged in</t>
@@ -820,6 +805,21 @@
   </si>
   <si>
     <t>SW033, SW036</t>
+  </si>
+  <si>
+    <t>Log in with invalid credentials.</t>
+  </si>
+  <si>
+    <t>Badge icon over the shopping cart when removing all products and the cart is empty.</t>
+  </si>
+  <si>
+    <t>1. Enter valid data in First Name field.
+2. Enter valid data in Last Name field.
+3. Leave Zip/Postal Code field empty.
+4. Press Continue button.</t>
+  </si>
+  <si>
+    <t>SW033B34:B37</t>
   </si>
 </sst>
 </file>
@@ -882,13 +882,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2000CD33-61D4-4DF7-A171-BA08DDF392FC}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1201,13 +1202,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1233,9 +1234,9 @@
     </row>
     <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1257,14 +1258,14 @@
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1286,30 +1287,30 @@
         <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -1317,25 +1318,25 @@
     </row>
     <row r="5" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
@@ -1343,25 +1344,25 @@
     </row>
     <row r="6" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -1369,28 +1370,28 @@
     </row>
     <row r="7" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
@@ -1398,28 +1399,28 @@
     </row>
     <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
@@ -1427,28 +1428,28 @@
     </row>
     <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
@@ -1456,28 +1457,28 @@
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
@@ -1485,28 +1486,28 @@
     </row>
     <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
@@ -1514,28 +1515,28 @@
     </row>
     <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
@@ -1543,28 +1544,28 @@
     </row>
     <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
+        <v>46</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
@@ -1572,28 +1573,28 @@
     </row>
     <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
@@ -1601,28 +1602,28 @@
     </row>
     <row r="15" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
@@ -1630,28 +1631,28 @@
     </row>
     <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
@@ -1659,28 +1660,28 @@
     </row>
     <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
@@ -1688,28 +1689,28 @@
     </row>
     <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
@@ -1717,28 +1718,28 @@
     </row>
     <row r="19" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
@@ -1746,28 +1747,28 @@
     </row>
     <row r="20" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="F20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
@@ -1775,28 +1776,28 @@
     </row>
     <row r="21" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
@@ -1804,28 +1805,28 @@
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
@@ -1833,28 +1834,28 @@
     </row>
     <row r="23" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
+        <v>51</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
@@ -1862,28 +1863,28 @@
     </row>
     <row r="24" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
@@ -1891,28 +1892,28 @@
     </row>
     <row r="25" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
@@ -1920,28 +1921,28 @@
     </row>
     <row r="26" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
@@ -1949,28 +1950,28 @@
     </row>
     <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
+        <v>51</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
@@ -1978,28 +1979,28 @@
     </row>
     <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
+        <v>53</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
@@ -2007,28 +2008,28 @@
     </row>
     <row r="29" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
@@ -2036,28 +2037,28 @@
     </row>
     <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>108</v>
+        <v>55</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
@@ -2065,28 +2066,28 @@
     </row>
     <row r="31" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>109</v>
+        <v>56</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
@@ -2094,28 +2095,28 @@
     </row>
     <row r="32" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>156</v>
+        <v>57</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
@@ -2123,28 +2124,28 @@
     </row>
     <row r="33" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>173</v>
+        <v>58</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
@@ -2152,28 +2153,28 @@
     </row>
     <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
@@ -2181,83 +2182,83 @@
     </row>
     <row r="35" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="203" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B36" t="s">
-        <v>204</v>
+        <v>209</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="232" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -2466,10 +2467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B510231E-BF2B-4144-A3DB-453E099D7522}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2480,23 +2481,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -2504,7 +2505,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -2512,7 +2513,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -2520,131 +2521,134 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>224</v>
-      </c>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>